<commit_message>
adjustments for calibration and coverage (for 3 RokiG scenarios)
</commit_message>
<xml_diff>
--- a/docs/data_prep/scenario_design/Scenario_InputTables.xlsx
+++ b/docs/data_prep/scenario_design/Scenario_InputTables.xlsx
@@ -1,25 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25221DB-32EE-45F2-8D44-5268982058E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="4545"/>
+    <workbookView xWindow="38280" yWindow="-135" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="94">
   <si>
     <t>Table Name</t>
   </si>
@@ -84,9 +96,6 @@
     <t>Already scenario-dependent</t>
   </si>
   <si>
-    <t>Scenario_Building_UnitArea.xlsx</t>
-  </si>
-  <si>
     <t>Scenario_BuildingComponent_Input_Labor.xlsx</t>
   </si>
   <si>
@@ -210,9 +219,6 @@
     <t>Scenario_UnitUser.xlsx</t>
   </si>
   <si>
-    <t>Scenario_UsefulEnergyDemandIndex_ApplianceElectricity.xlsx</t>
-  </si>
-  <si>
     <t>Scenario_BuildingComponent_Cost_Material.xlsx</t>
   </si>
   <si>
@@ -228,9 +234,6 @@
     <t>5 years later than 1 for everything (after 2025)</t>
   </si>
   <si>
-    <t>can we make sure serial renovation is not available since 1900 somehow?</t>
-  </si>
-  <si>
     <t>50% lower than conventional (id_building_action=2) after 2025</t>
   </si>
   <si>
@@ -249,21 +252,12 @@
     <t>fix typo in table name</t>
   </si>
   <si>
-    <t>is thisthe table to apply overall efficiency gains in tech.?</t>
-  </si>
-  <si>
     <t>not applicable</t>
   </si>
   <si>
-    <t>is this relevant for living space as described in Category 5 (--&gt; increasing single-person households and thus,higher demand of living space)? and/or, should I increase Scenario_Building_UnitArea in parallel?</t>
-  </si>
-  <si>
     <t>Scenario_Construction_MandatoryRenewableHeating.xlsx</t>
   </si>
   <si>
-    <t>should it be dependent on action type (i.e. conventional and serial?) --&gt; if we want to push for more serial renovation and the costs for serial renovation are higher, this might be the only lever to increase serial renovation + the master thesis student said that there are 15% additional subsidies for serial renovation anyway</t>
-  </si>
-  <si>
     <t>for id_action = 1&amp;2</t>
   </si>
   <si>
@@ -280,12 +274,51 @@
   </si>
   <si>
     <t>made scenario-dependent, with code changes (19.08.2024)</t>
+  </si>
+  <si>
+    <t>is this relevant for living space as described in Category 5 (--&gt; increasing single-person households and thus, higher demand of living space)? and/or, should I increase Scenario_Building_UnitArea in parallel?</t>
+  </si>
+  <si>
+    <t>check FLEX-Summary file from Songmin for plausible rates</t>
+  </si>
+  <si>
+    <t>same 1</t>
+  </si>
+  <si>
+    <t>medium efficiency increase</t>
+  </si>
+  <si>
+    <t>ambitious efficiency increase</t>
+  </si>
+  <si>
+    <t>also vary the non-electricity energy carriers demand by ambition level of scenario</t>
+  </si>
+  <si>
+    <t>increasing single-person households (1) and reducing type 2 and 5 at the same time.</t>
+  </si>
+  <si>
+    <t>make sure total population is consistent</t>
+  </si>
+  <si>
+    <t>increasing type 2 and 5, and reducing single-person households (1) at the same time.</t>
+  </si>
+  <si>
+    <t>check again if there is any data. if not, and if we still want to include conclusions about low-temp DH readiness, we could show our assumptions and say that there is no historic data, but these are our assumptions.</t>
+  </si>
+  <si>
+    <t>not considered for RokiG</t>
+  </si>
+  <si>
+    <t>it should be dependent on action type (i.e. conventional and serial) --&gt; if we want to push for more serial renovation and the costs for serial renovation are higher, this might be the only lever to increase serial renovation + the master thesis student said that there are 15% additional subsidies for serial renovation anyway</t>
+  </si>
+  <si>
+    <t>can we make sure serial renovation is not available since 1900 somehow? --&gt; yes, in code, historic renovation can happen only by conventional. only for future, serial renovation is an option. additionally, we can also make the availability table 0 for action_type=3 until 2024.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -303,7 +336,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,6 +367,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -347,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -376,9 +415,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,7 +457,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -702,20 +751,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="3" max="4" width="78.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="74.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -723,24 +771,24 @@
         <v>0</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="9"/>
       <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="F2" s="12"/>
     </row>
@@ -773,13 +821,13 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F6" s="7"/>
     </row>
@@ -803,13 +851,13 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="7"/>
     </row>
@@ -819,13 +867,13 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="7"/>
     </row>
@@ -835,13 +883,13 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="7"/>
     </row>
@@ -851,13 +899,13 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="7"/>
     </row>
@@ -867,13 +915,13 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="7"/>
     </row>
@@ -883,13 +931,13 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
         <v>31</v>
       </c>
-      <c r="D14" t="s">
-        <v>32</v>
-      </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" s="7"/>
     </row>
@@ -899,13 +947,13 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
         <v>33</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>34</v>
-      </c>
-      <c r="E15" t="s">
-        <v>35</v>
       </c>
       <c r="F15" s="7"/>
     </row>
@@ -915,13 +963,13 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
         <v>37</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>38</v>
-      </c>
-      <c r="E16" t="s">
-        <v>39</v>
       </c>
       <c r="F16" s="7"/>
     </row>
@@ -931,13 +979,13 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F17" s="7"/>
     </row>
@@ -947,13 +995,13 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" s="7"/>
     </row>
@@ -963,13 +1011,13 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F19" s="7"/>
     </row>
@@ -979,16 +1027,16 @@
         <v>18</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="F20" s="7" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -997,124 +1045,124 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" t="s">
         <v>59</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>60</v>
       </c>
-      <c r="E21" t="s">
-        <v>61</v>
-      </c>
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>86</v>
+      <c r="A22" s="14" t="s">
+        <v>80</v>
       </c>
       <c r="B22" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" t="s">
         <v>64</v>
       </c>
-      <c r="C22" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>81</v>
+      <c r="F22" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="13"/>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D23" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E23" t="s">
-        <v>85</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="F23" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>70</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" t="s">
         <v>71</v>
       </c>
-      <c r="E24" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" t="s">
-        <v>74</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" t="s">
-        <v>74</v>
-      </c>
       <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
+      <c r="A27" s="14"/>
       <c r="B27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
         <v>40</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>41</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>42</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="C28" s="6">
         <v>0.5</v>
@@ -1125,135 +1173,146 @@
       <c r="E28" s="6">
         <v>0.15</v>
       </c>
-      <c r="F28" s="7"/>
+      <c r="F28" s="7" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="B29" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" t="s">
+        <v>83</v>
+      </c>
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>53</v>
+      <c r="B30" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" t="s">
+        <v>87</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>88</v>
       </c>
       <c r="G30" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G31" t="s">
-        <v>76</v>
+      <c r="B31" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C32" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D32" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" t="s">
-        <v>46</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
+      <c r="C33" t="s">
         <v>45</v>
       </c>
-      <c r="C33" t="s">
-        <v>46</v>
-      </c>
       <c r="D33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="G33" s="17"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C34" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" t="s">
-        <v>46</v>
-      </c>
-      <c r="E34" t="s">
-        <v>46</v>
-      </c>
       <c r="F34" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="B37" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="B36" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="F38" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="G32:G33"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A3:A21"/>

</xml_diff>

<commit_message>
future weather projections are added. heating tech. availabilities are adjusted for RokiG scenarios and hydrogen heating technology in base year is fixed.
</commit_message>
<xml_diff>
--- a/docs/data_prep/scenario_design/Scenario_InputTables.xlsx
+++ b/docs/data_prep/scenario_design/Scenario_InputTables.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25221DB-32EE-45F2-8D44-5268982058E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-135" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-135" windowWidth="38640" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="95">
   <si>
     <t>Table Name</t>
   </si>
@@ -129,15 +128,6 @@
     <t>65% after 2025</t>
   </si>
   <si>
-    <t>no oil boilers allowed after 2025, no (natural) gas boilers allowed after 2035</t>
-  </si>
-  <si>
-    <t>no oil boilers allowed after 2030, no (natural) gas boilers allowed after 2040</t>
-  </si>
-  <si>
-    <t>no oil boilers allowed after 2035, no (natural) gas boilers allowed after 2045</t>
-  </si>
-  <si>
     <t>Scenario_HeatingTechnology_EfficiencyCoefficient.xlsx</t>
   </si>
   <si>
@@ -313,13 +303,25 @@
   </si>
   <si>
     <t>can we make sure serial renovation is not available since 1900 somehow? --&gt; yes, in code, historic renovation can happen only by conventional. only for future, serial renovation is an option. additionally, we can also make the availability table 0 for action_type=3 until 2024.</t>
+  </si>
+  <si>
+    <t>not fully effective for now as we don't have complicated combinations of fossil and renewable heating technologies. for now, we only have solar thermal and electric heater that decides the RE share and they are usually not very large to make the total share reach above 50%</t>
+  </si>
+  <si>
+    <t>no fossil boilers allowed after 2025</t>
+  </si>
+  <si>
+    <t>no fossil boilers allowed after 2035</t>
+  </si>
+  <si>
+    <t>no fossil boilers allowed after 2045</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +333,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -386,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -397,6 +406,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -418,11 +432,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,11 +762,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,20 +778,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="12" t="s">
-        <v>51</v>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="9"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="1" t="s">
         <v>24</v>
       </c>
@@ -790,10 +801,10 @@
       <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="12"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="13" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -802,51 +813,51 @@
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -862,7 +873,7 @@
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -878,7 +889,7 @@
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
@@ -894,7 +905,7 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
@@ -910,7 +921,7 @@
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
@@ -926,55 +937,57 @@
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="13"/>
+      <c r="B14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="7" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
@@ -990,7 +1003,7 @@
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1006,163 +1019,163 @@
       <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E21" t="s">
+      <c r="C22" t="s">
         <v>60</v>
       </c>
-      <c r="F21" s="7"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" t="s">
-        <v>63</v>
-      </c>
       <c r="D22" t="s">
         <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="16"/>
+      <c r="C23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="13"/>
-      <c r="C23" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" t="s">
-        <v>78</v>
-      </c>
       <c r="E23" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
+      <c r="B25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" t="s">
         <v>67</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F25" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" t="s">
         <v>39</v>
       </c>
-      <c r="C27" t="s">
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="D27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E27" t="s">
-        <v>42</v>
-      </c>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="C28" s="6">
         <v>0.5</v>
@@ -1174,140 +1187,140 @@
         <v>0.15</v>
       </c>
       <c r="F28" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" t="s">
+        <v>84</v>
+      </c>
+      <c r="F30" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D29" t="s">
-        <v>84</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="G30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" t="s">
-        <v>89</v>
-      </c>
-      <c r="D30" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" t="s">
-        <v>87</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="G30" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" t="s">
-        <v>85</v>
-      </c>
-      <c r="D31" t="s">
-        <v>84</v>
-      </c>
-      <c r="E31" t="s">
-        <v>83</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D32" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E32" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G32" s="17" t="s">
-        <v>90</v>
+        <v>49</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D33" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E33" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G33" s="17"/>
+        <v>49</v>
+      </c>
+      <c r="G33" s="10"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F34" s="7" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
+      <c r="A35" s="14"/>
       <c r="B35" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
+      <c r="A36" s="14"/>
       <c r="B36" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
+      <c r="A37" s="14"/>
       <c r="B37" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scenario pathways for unit user composition in line with eurostat population projections are added. heating technology efficiency gains are also made scenario-dependent.
</commit_message>
<xml_diff>
--- a/docs/data_prep/scenario_design/Scenario_InputTables.xlsx
+++ b/docs/data_prep/scenario_design/Scenario_InputTables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F304803-0779-4039-9B98-B67985DAE7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-135" windowWidth="38640" windowHeight="21240"/>
+    <workbookView xWindow="28680" yWindow="1560" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="97">
   <si>
     <t>Table Name</t>
   </si>
@@ -239,9 +240,6 @@
     <t>not mandatory</t>
   </si>
   <si>
-    <t>fix typo in table name</t>
-  </si>
-  <si>
     <t>not applicable</t>
   </si>
   <si>
@@ -272,9 +270,6 @@
     <t>check FLEX-Summary file from Songmin for plausible rates</t>
   </si>
   <si>
-    <t>same 1</t>
-  </si>
-  <si>
     <t>medium efficiency increase</t>
   </si>
   <si>
@@ -302,9 +297,6 @@
     <t>it should be dependent on action type (i.e. conventional and serial) --&gt; if we want to push for more serial renovation and the costs for serial renovation are higher, this might be the only lever to increase serial renovation + the master thesis student said that there are 15% additional subsidies for serial renovation anyway</t>
   </si>
   <si>
-    <t>can we make sure serial renovation is not available since 1900 somehow? --&gt; yes, in code, historic renovation can happen only by conventional. only for future, serial renovation is an option. additionally, we can also make the availability table 0 for action_type=3 until 2024.</t>
-  </si>
-  <si>
     <t>not fully effective for now as we don't have complicated combinations of fossil and renewable heating technologies. for now, we only have solar thermal and electric heater that decides the RE share and they are usually not very large to make the total share reach above 50%</t>
   </si>
   <si>
@@ -315,12 +307,27 @@
   </si>
   <si>
     <t>no fossil boilers allowed after 2045</t>
+  </si>
+  <si>
+    <t>make scenario-dependent</t>
+  </si>
+  <si>
+    <t>fixed typo in table name</t>
+  </si>
+  <si>
+    <t>additionally, we can also make the availability table 0 for action_type=3 until 2024.</t>
+  </si>
+  <si>
+    <t>make sure serial renovation is not available since 1900? --&gt; yes, in code, historic renovation can happen only by conventional. only for future, serial renovation is an option.</t>
+  </si>
+  <si>
+    <t>only for heat pumps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -406,11 +413,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -432,8 +440,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -762,11 +777,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,20 +793,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="15" t="s">
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="16" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="12"/>
+      <c r="B2" s="13"/>
       <c r="C2" s="1" t="s">
         <v>24</v>
       </c>
@@ -801,10 +816,10 @@
       <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="15"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -813,21 +828,21 @@
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -843,21 +858,21 @@
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -873,7 +888,7 @@
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -889,7 +904,7 @@
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
@@ -905,7 +920,7 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
@@ -921,7 +936,7 @@
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
@@ -937,41 +952,41 @@
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="18" t="s">
+      <c r="A14" s="14"/>
+      <c r="B14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>91</v>
+      <c r="F14" s="19" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
@@ -987,7 +1002,7 @@
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1003,7 +1018,7 @@
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1019,23 +1034,23 @@
       <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1048,12 +1063,12 @@
       <c r="E20" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="7" t="s">
-        <v>89</v>
+      <c r="F20" s="21" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1069,81 +1084,84 @@
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" s="16" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>60</v>
       </c>
-      <c r="D22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" t="s">
         <v>61</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="17"/>
+      <c r="C24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="16"/>
-      <c r="C23" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23" t="s">
-        <v>76</v>
-      </c>
-      <c r="F23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="3" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>64</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>65</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>66</v>
       </c>
-      <c r="F24" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>69</v>
+      <c r="F25" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="3" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="C26" t="s">
         <v>67</v>
@@ -1151,95 +1169,102 @@
       <c r="D26" t="s">
         <v>67</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="20" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>37</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>38</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E28" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="3" t="s">
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
+      <c r="B29" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C29" s="6">
         <v>0.5</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D29" s="6">
         <v>0.3</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E29" s="6">
         <v>0.15</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F29" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" t="s">
+        <v>83</v>
+      </c>
+      <c r="G30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
+      <c r="B31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="E31" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" t="s">
         <v>81</v>
-      </c>
-      <c r="E29" t="s">
-        <v>80</v>
-      </c>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" t="s">
-        <v>84</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G30" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" t="s">
-        <v>81</v>
-      </c>
-      <c r="E31" t="s">
-        <v>80</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1258,8 +1283,8 @@
       <c r="F32" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G32" s="10" t="s">
-        <v>87</v>
+      <c r="G32" s="22" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1278,7 +1303,7 @@
       <c r="F33" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G33" s="10"/>
+      <c r="G33" s="22"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
@@ -1289,7 +1314,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="4" t="s">
         <v>45</v>
       </c>
@@ -1298,7 +1323,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="4" t="s">
         <v>46</v>
       </c>
@@ -1307,7 +1332,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="4" t="s">
         <v>51</v>
       </c>
@@ -1319,20 +1344,21 @@
       <c r="B38" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F38" s="7" t="s">
-        <v>88</v>
+      <c r="F38" s="19" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="G32:G33"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A3:A21"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A23:A29"/>
+    <mergeCell ref="A30:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>